<commit_message>
- Incorporated ZW model - Moved objects to database - Renamed models - Added new database: support.db - Amended bulk upload template
</commit_message>
<xml_diff>
--- a/App/uap_cross_sell/www/files/cs_upload_template.xlsx
+++ b/App/uap_cross_sell/www/files/cs_upload_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Contracts\UAP\D - Working Papers\UAP-cross-sell\App\uap_cross_sell\www\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E2B0734-D689-4E65-9067-60841AF24642}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A70AE80-7A1B-438A-9743-A2FFA9E6F04E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{24700C77-9C92-4468-B9C5-B77420552ACF}"/>
   </bookViews>
@@ -17,6 +17,10 @@
     <sheet name="customer_prod" sheetId="2" r:id="rId2"/>
     <sheet name="valid_product_names" sheetId="3" state="hidden" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="Kenya">valid_product_names!$A$2:$A$62</definedName>
+    <definedName name="Zimbabwe">valid_product_names!$B$2:$B$9</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -27,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="74">
   <si>
     <t>Old Mutual Equity Fund</t>
   </si>
@@ -216,6 +220,39 @@
   </si>
   <si>
     <t>MONEY-PLUS_MP</t>
+  </si>
+  <si>
+    <t>Kenya</t>
+  </si>
+  <si>
+    <t>Fixed Interest - Money Market</t>
+  </si>
+  <si>
+    <t>Equity - General</t>
+  </si>
+  <si>
+    <t>Real Estate - General</t>
+  </si>
+  <si>
+    <t>Flexi Funeral Plan</t>
+  </si>
+  <si>
+    <t>Funeral Plan</t>
+  </si>
+  <si>
+    <t>Term Plan</t>
+  </si>
+  <si>
+    <t>Life Plan</t>
+  </si>
+  <si>
+    <t>Savings Plan</t>
+  </si>
+  <si>
+    <t>Zimbabwe</t>
+  </si>
+  <si>
+    <t>SELECT A COUNTRY</t>
   </si>
 </sst>
 </file>
@@ -607,9 +644,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C783F41-9AF8-4698-A4E2-A0CDF8EF2C34}">
-  <dimension ref="A1:A20"/>
+  <dimension ref="A1:A19"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -633,11 +672,13 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <v>1397</v>
+        <v>100003</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
+      <c r="A5" s="2">
+        <v>101403</v>
+      </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
@@ -680,9 +721,6 @@
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -691,85 +729,105 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A24E3401-6C35-4108-BA35-AB6F39FFE1F7}">
-  <dimension ref="A1:A16"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C1" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
     </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+    </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A19" xr:uid="{168CF669-CF3F-4DD2-90BE-158AF429FF0F}">
+      <formula1>INDIRECT($C$2)</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select a product from the drop down below." xr:uid="{477D1398-E957-4CC1-AC67-53ED8644704C}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F06FDF89-FCC4-438E-B054-39500F380DC7}">
           <x14:formula1>
-            <xm:f>valid_product_names!$A:$A</xm:f>
+            <xm:f>valid_product_names!$A$1:$B$1</xm:f>
           </x14:formula1>
-          <xm:sqref>A2:A16</xm:sqref>
+          <xm:sqref>C2</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -779,316 +837,352 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35D5C44B-F88A-4340-B982-5E1C9A94327D}">
-  <dimension ref="A1:A61"/>
+  <dimension ref="A1:B62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="37" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="B9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
         <v>62</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Included ZW General Insurance and Lending business lines.
</commit_message>
<xml_diff>
--- a/App/uap_cross_sell/www/files/cs_upload_template.xlsx
+++ b/App/uap_cross_sell/www/files/cs_upload_template.xlsx
@@ -8,18 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Contracts\UAP\D - Working Papers\UAP-cross-sell\App\uap_cross_sell\www\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A70AE80-7A1B-438A-9743-A2FFA9E6F04E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AC88076-9593-4CDC-BE41-31DCBA16B2D4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{24700C77-9C92-4468-B9C5-B77420552ACF}"/>
   </bookViews>
   <sheets>
     <sheet name="customer_acc" sheetId="1" r:id="rId1"/>
     <sheet name="customer_prod" sheetId="2" r:id="rId2"/>
-    <sheet name="valid_product_names" sheetId="3" state="hidden" r:id="rId3"/>
+    <sheet name="valid_product_names" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="Kenya">valid_product_names!$A$2:$A$62</definedName>
-    <definedName name="Zimbabwe">valid_product_names!$B$2:$B$9</definedName>
+    <definedName name="Zimbabwe">valid_product_names!$B$2:$B$68</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="133">
   <si>
     <t>Old Mutual Equity Fund</t>
   </si>
@@ -253,6 +253,183 @@
   </si>
   <si>
     <t>SELECT A COUNTRY</t>
+  </si>
+  <si>
+    <t>Agribusiness Loan</t>
+  </si>
+  <si>
+    <t>Working Capital Loans- Group Clients</t>
+  </si>
+  <si>
+    <t>Order Finance Loans</t>
+  </si>
+  <si>
+    <t>Working Capital Loans- Individual clients (Unsecured loans)</t>
+  </si>
+  <si>
+    <t>Salary Based Loan</t>
+  </si>
+  <si>
+    <t>Structured Finance Loan</t>
+  </si>
+  <si>
+    <t>SOFL</t>
+  </si>
+  <si>
+    <t>SFN</t>
+  </si>
+  <si>
+    <t>HOME PLAN</t>
+  </si>
+  <si>
+    <t>Private Motor Car</t>
+  </si>
+  <si>
+    <t>Personal Package</t>
+  </si>
+  <si>
+    <t>PTA Yellow Card</t>
+  </si>
+  <si>
+    <t>Motor Combined</t>
+  </si>
+  <si>
+    <t>Motor Act</t>
+  </si>
+  <si>
+    <t>Motor Fleet</t>
+  </si>
+  <si>
+    <t>Business Package</t>
+  </si>
+  <si>
+    <t>Employers Personal Accident</t>
+  </si>
+  <si>
+    <t>Assets All Risks</t>
+  </si>
+  <si>
+    <t>Employers/Residual Liability</t>
+  </si>
+  <si>
+    <t>Fronting Product</t>
+  </si>
+  <si>
+    <t>Liabilities</t>
+  </si>
+  <si>
+    <t>Machinery Breakdown</t>
+  </si>
+  <si>
+    <t>Marine Cargo</t>
+  </si>
+  <si>
+    <t>MOTOR PLAN</t>
+  </si>
+  <si>
+    <t>Marine Hull</t>
+  </si>
+  <si>
+    <t>Bonds - Court</t>
+  </si>
+  <si>
+    <t>Personal Combined: Old Mutual</t>
+  </si>
+  <si>
+    <t>CABS</t>
+  </si>
+  <si>
+    <t>Fidelity Guarantee</t>
+  </si>
+  <si>
+    <t>Houseowners</t>
+  </si>
+  <si>
+    <t>Contractors</t>
+  </si>
+  <si>
+    <t>Personal Accident</t>
+  </si>
+  <si>
+    <t>Marine Open Policy</t>
+  </si>
+  <si>
+    <t>Motor Fleet Eaton &amp; Young</t>
+  </si>
+  <si>
+    <t>Farmers Package</t>
+  </si>
+  <si>
+    <t>Personal Combined: RMI</t>
+  </si>
+  <si>
+    <t>Zimbabwe Caravan Association</t>
+  </si>
+  <si>
+    <t>SME Business Package</t>
+  </si>
+  <si>
+    <t>Kingsure Personal Package</t>
+  </si>
+  <si>
+    <t>Fire</t>
+  </si>
+  <si>
+    <t>Machinery Loss of Profits</t>
+  </si>
+  <si>
+    <t>Travel Insurance</t>
+  </si>
+  <si>
+    <t>Agrisure Personal Package</t>
+  </si>
+  <si>
+    <t>Professional Indemnity</t>
+  </si>
+  <si>
+    <t>Reinsurance For All Products</t>
+  </si>
+  <si>
+    <t>Motor Traders External</t>
+  </si>
+  <si>
+    <t>Livestock &amp; Bloodstock</t>
+  </si>
+  <si>
+    <t>MBCA Insure Motor Plan</t>
+  </si>
+  <si>
+    <t>MBCA Insure Home Plan</t>
+  </si>
+  <si>
+    <t>Mortgage Guarantee</t>
+  </si>
+  <si>
+    <t>Forex Travel Insurance</t>
+  </si>
+  <si>
+    <t>Aviation</t>
+  </si>
+  <si>
+    <t>Stanchart Personal Pcakage</t>
+  </si>
+  <si>
+    <t>Electronic Gadgets Insurance</t>
+  </si>
+  <si>
+    <t>Allsure</t>
+  </si>
+  <si>
+    <t>Emergency Rescue</t>
+  </si>
+  <si>
+    <t>Medic-Sure</t>
+  </si>
+  <si>
+    <t>Loss of Profits</t>
+  </si>
+  <si>
+    <t>Living Future</t>
   </si>
 </sst>
 </file>
@@ -732,7 +909,7 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -752,24 +929,26 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>65</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>3</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>26</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
+      <c r="A5" s="2" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
@@ -837,10 +1016,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35D5C44B-F88A-4340-B982-5E1C9A94327D}">
-  <dimension ref="A1:B62"/>
+  <dimension ref="A1:B68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B1" activeCellId="1" sqref="A1:A62 B1:B68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -862,7 +1041,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -870,7 +1049,7 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -878,7 +1057,7 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -886,7 +1065,7 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -894,7 +1073,7 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -902,7 +1081,7 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -910,7 +1089,7 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -918,272 +1097,461 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>2</v>
       </c>
+      <c r="B10" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
+      <c r="B11" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
+      <c r="B12" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
+      <c r="B13" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
+      <c r="B14" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
+      <c r="B15" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>62</v>
+      </c>
+      <c r="B62" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
+        <v>132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Removed null product - Included full products names for Lending
</commit_message>
<xml_diff>
--- a/App/uap_cross_sell/www/files/cs_upload_template.xlsx
+++ b/App/uap_cross_sell/www/files/cs_upload_template.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tayojabar/Documents/OML/UAP-cross-sell/UAP-cross-sell/App/uap_cross_sell/www/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Contracts\UAP\D - Working Papers\UAP-cross-sell\App\uap_cross_sell\www\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29BA7B76-E444-1E42-A2EC-67C033E61ED4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B39D9A0-A473-48DF-A5C2-94EA7611F2FA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{24700C77-9C92-4468-B9C5-B77420552ACF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{24700C77-9C92-4468-B9C5-B77420552ACF}"/>
   </bookViews>
   <sheets>
     <sheet name="customer_acc" sheetId="1" r:id="rId1"/>
     <sheet name="customer_prod" sheetId="2" r:id="rId2"/>
-    <sheet name="valid_product_names" sheetId="3" r:id="rId3"/>
+    <sheet name="valid_product_names" sheetId="3" state="hidden" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="Kenya">valid_product_names!$A$2:$A$62</definedName>
-    <definedName name="Uganda">valid_product_names!$C$2:$C$103</definedName>
-    <definedName name="Zimbabwe">valid_product_names!$B$2:$B$68</definedName>
+    <definedName name="Uganda">valid_product_names!$C$2:$C$102</definedName>
+    <definedName name="Zimbabwe">valid_product_names!$B$2:$B$62</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="221">
   <si>
     <t>Old Mutual Equity Fund</t>
   </si>
@@ -256,9 +256,6 @@
     <t>SELECT A COUNTRY</t>
   </si>
   <si>
-    <t>Agribusiness Loan</t>
-  </si>
-  <si>
     <t>Working Capital Loans- Group Clients</t>
   </si>
   <si>
@@ -268,18 +265,9 @@
     <t>Working Capital Loans- Individual clients (Unsecured loans)</t>
   </si>
   <si>
-    <t>Salary Based Loan</t>
-  </si>
-  <si>
     <t>Structured Finance Loan</t>
   </si>
   <si>
-    <t>SOFL</t>
-  </si>
-  <si>
-    <t>SFN</t>
-  </si>
-  <si>
     <t>HOME PLAN</t>
   </si>
   <si>
@@ -364,15 +352,9 @@
     <t>Personal Combined: RMI</t>
   </si>
   <si>
-    <t>Zimbabwe Caravan Association</t>
-  </si>
-  <si>
     <t>SME Business Package</t>
   </si>
   <si>
-    <t>Kingsure Personal Package</t>
-  </si>
-  <si>
     <t>Fire</t>
   </si>
   <si>
@@ -382,9 +364,6 @@
     <t>Travel Insurance</t>
   </si>
   <si>
-    <t>Agrisure Personal Package</t>
-  </si>
-  <si>
     <t>Professional Indemnity</t>
   </si>
   <si>
@@ -412,21 +391,9 @@
     <t>Aviation</t>
   </si>
   <si>
-    <t>Stanchart Personal Pcakage</t>
-  </si>
-  <si>
     <t>Electronic Gadgets Insurance</t>
   </si>
   <si>
-    <t>Allsure</t>
-  </si>
-  <si>
-    <t>Emergency Rescue</t>
-  </si>
-  <si>
-    <t>Medic-Sure</t>
-  </si>
-  <si>
     <t>Loss of Profits</t>
   </si>
   <si>
@@ -484,9 +451,6 @@
     <t>MAXILLOFACIAL AND ORAL SURGERY</t>
   </si>
   <si>
-    <t>NULL</t>
-  </si>
-  <si>
     <t>OPTHALMOLOGY</t>
   </si>
   <si>
@@ -716,6 +680,21 @@
   </si>
   <si>
     <t>LIVESTOCK</t>
+  </si>
+  <si>
+    <t>Agriculture Business Loan</t>
+  </si>
+  <si>
+    <t>Salary Based Loans - Salaried Individuals</t>
+  </si>
+  <si>
+    <t>School Fees Loans</t>
+  </si>
+  <si>
+    <t>Working Capital Loans- Individual clients (secured loans)</t>
+  </si>
+  <si>
+    <t>Structured Order Finance Loan</t>
   </si>
 </sst>
 </file>
@@ -1113,80 +1092,80 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1537</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1418</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>100003</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>101403</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>1016908</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>1024783</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
     </row>
   </sheetData>
@@ -1199,17 +1178,17 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
@@ -1217,71 +1196,71 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
     </row>
   </sheetData>
@@ -1308,19 +1287,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35D5C44B-F88A-4340-B982-5E1C9A94327D}">
-  <dimension ref="A1:C103"/>
+  <dimension ref="A1:C102"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" activeCellId="2" sqref="A1:A62 B1:B68 C1:C103"/>
+      <selection activeCell="C1" activeCellId="2" sqref="A1:A62 B1:B62 C1:C102"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="56.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>63</v>
       </c>
@@ -1328,10 +1308,10 @@
         <v>72</v>
       </c>
       <c r="C1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1339,890 +1319,867 @@
         <v>67</v>
       </c>
       <c r="C2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>74</v>
+        <v>216</v>
       </c>
       <c r="C3" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C4" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C5" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C6" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>78</v>
+        <v>217</v>
       </c>
       <c r="C7" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>79</v>
+        <v>218</v>
       </c>
       <c r="C8" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>80</v>
+        <v>219</v>
       </c>
       <c r="C9" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>81</v>
+        <v>220</v>
       </c>
       <c r="C10" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="C11" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C12" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C13" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C14" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="C15" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C16" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C17" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="C18" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C19" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C20" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C21" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C22" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C23" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C24" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C25" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C26" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C27" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C28" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C29" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>30</v>
       </c>
       <c r="B30" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C30" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>31</v>
       </c>
       <c r="B31" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C31" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C32" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>33</v>
       </c>
       <c r="B33" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C33" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>34</v>
       </c>
       <c r="B34" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C34" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C35" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>36</v>
       </c>
       <c r="B36" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C36" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>37</v>
       </c>
       <c r="B37" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C37" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>38</v>
       </c>
       <c r="B38" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="C38" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>39</v>
       </c>
       <c r="B39" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="C39" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>40</v>
       </c>
       <c r="B40" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C40" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>41</v>
       </c>
       <c r="B41" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C41" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>42</v>
       </c>
       <c r="B42" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C42" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>43</v>
       </c>
       <c r="B43" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C43" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>44</v>
       </c>
       <c r="B44" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C44" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>45</v>
       </c>
       <c r="B45" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C45" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>46</v>
       </c>
       <c r="B46" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C46" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>47</v>
       </c>
       <c r="B47" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C47" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>48</v>
       </c>
       <c r="B48" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C48" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>49</v>
       </c>
       <c r="B49" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="C49" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>50</v>
       </c>
       <c r="B50" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C50" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>51</v>
       </c>
       <c r="B51" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="C51" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>52</v>
       </c>
       <c r="B52" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C52" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>53</v>
       </c>
       <c r="B53" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="C53" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>54</v>
       </c>
       <c r="B54" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C54" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>55</v>
       </c>
       <c r="B55" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C55" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>56</v>
       </c>
       <c r="B56" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C56" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>57</v>
       </c>
       <c r="B57" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C57" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>58</v>
       </c>
       <c r="B58" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="C58" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>59</v>
       </c>
       <c r="B59" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C59" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>60</v>
       </c>
       <c r="B60" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C60" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>61</v>
       </c>
       <c r="B61" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="C61" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>62</v>
       </c>
       <c r="B62" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C62" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B63" t="s">
-        <v>127</v>
-      </c>
+        <v>181</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C63" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C64" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="65" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C65" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="66" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C66" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="67" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C67" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="68" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C68" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="69" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C69" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="70" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C70" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="71" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C71" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="72" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C72" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="73" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C73" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="74" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C74" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="75" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C75" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="76" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C76" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="77" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C77" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B64" t="s">
-        <v>128</v>
-      </c>
-      <c r="C64" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B65" t="s">
-        <v>129</v>
-      </c>
-      <c r="C65" t="s">
+    <row r="78" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C78" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="66" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B66" t="s">
-        <v>130</v>
-      </c>
-      <c r="C66" t="s">
+    <row r="79" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C79" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="80" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C80" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="67" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B67" t="s">
-        <v>131</v>
-      </c>
-      <c r="C67" t="s">
+    <row r="81" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C81" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="68" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B68" t="s">
-        <v>132</v>
-      </c>
-      <c r="C68" t="s">
+    <row r="82" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C82" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="83" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C83" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="84" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C84" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="69" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C69" t="s">
+    <row r="85" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C85" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="70" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C70" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="71" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C71" t="s">
+    <row r="86" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C86" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="72" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C72" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="73" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C73" t="s">
+    <row r="87" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C87" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="74" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C74" t="s">
+    <row r="88" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C88" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="75" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C75" t="s">
+    <row r="89" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C89" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="76" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C76" t="s">
+    <row r="90" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C90" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="77" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C77" t="s">
+    <row r="91" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C91" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="78" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C78" t="s">
+    <row r="92" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C92" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="79" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C79" t="s">
+    <row r="93" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C93" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="80" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C80" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="81" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C81" t="s">
+    <row r="94" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C94" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="82" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C82" t="s">
+    <row r="95" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C95" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="83" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C83" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="84" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C84" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="85" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C85" t="s">
+    <row r="96" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C96" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="86" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C86" t="s">
+    <row r="97" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C97" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="87" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C87" t="s">
+    <row r="98" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C98" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="88" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C88" t="s">
+    <row r="99" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C99" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="89" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C89" t="s">
+    <row r="100" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C100" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="90" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C90" t="s">
+    <row r="101" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C101" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="91" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C91" t="s">
+    <row r="102" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C102" t="s">
         <v>215</v>
-      </c>
-    </row>
-    <row r="92" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C92" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="93" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C93" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="94" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C94" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="95" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C95" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="96" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C96" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="97" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C97" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="98" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C98" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="99" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C99" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="100" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C100" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="101" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C101" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="102" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C102" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="103" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C103" t="s">
-        <v>227</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Incorporated UG into the tool.
</commit_message>
<xml_diff>
--- a/App/uap_cross_sell/www/files/cs_upload_template.xlsx
+++ b/App/uap_cross_sell/www/files/cs_upload_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Contracts\UAP\D - Working Papers\UAP-cross-sell\App\uap_cross_sell\www\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B39D9A0-A473-48DF-A5C2-94EA7611F2FA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2B17867-B4A3-45FB-A13E-5888156D3F81}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{24700C77-9C92-4468-B9C5-B77420552ACF}"/>
   </bookViews>
@@ -19,7 +19,7 @@
   </sheets>
   <definedNames>
     <definedName name="Kenya">valid_product_names!$A$2:$A$62</definedName>
-    <definedName name="Uganda">valid_product_names!$C$2:$C$102</definedName>
+    <definedName name="Uganda">valid_product_names!$C$2:$C$97</definedName>
     <definedName name="Zimbabwe">valid_product_names!$B$2:$B$62</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="216">
   <si>
     <t>Old Mutual Equity Fund</t>
   </si>
@@ -664,22 +664,7 @@
     <t>SURETY UNDERTAKING</t>
   </si>
   <si>
-    <t>L.O.P. FOLLOWING MACHINERY B/DOWN</t>
-  </si>
-  <si>
     <t>MARINE HULL</t>
-  </si>
-  <si>
-    <t>RETENTION BOND</t>
-  </si>
-  <si>
-    <t>AVIATION</t>
-  </si>
-  <si>
-    <t>GOLFERS INSURANCE</t>
-  </si>
-  <si>
-    <t>LIVESTOCK</t>
   </si>
   <si>
     <t>Agriculture Business Loan</t>
@@ -1178,7 +1163,7 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1198,7 +1183,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>122</v>
@@ -1206,23 +1191,19 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>213</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>206</v>
-      </c>
+      <c r="A5" s="2"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>132</v>
-      </c>
+      <c r="A6" s="2"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
@@ -1287,10 +1268,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35D5C44B-F88A-4340-B982-5E1C9A94327D}">
-  <dimension ref="A1:C102"/>
+  <dimension ref="A1:C97"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" activeCellId="2" sqref="A1:A62 B1:B62 C1:C102"/>
+      <selection activeCell="C1" activeCellId="2" sqref="A1:A62 B1:B62 C1:C97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1319,7 +1300,7 @@
         <v>67</v>
       </c>
       <c r="C2" t="s">
-        <v>123</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1327,10 +1308,10 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="C3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1363,7 +1344,7 @@
         <v>76</v>
       </c>
       <c r="C6" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1371,10 +1352,10 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="C7" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1382,10 +1363,10 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="C8" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -1393,10 +1374,10 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="C9" t="s">
-        <v>130</v>
+        <v>153</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -1404,10 +1385,10 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="C10" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1418,7 +1399,7 @@
         <v>77</v>
       </c>
       <c r="C11" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1429,7 +1410,7 @@
         <v>71</v>
       </c>
       <c r="C12" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1440,7 +1421,7 @@
         <v>70</v>
       </c>
       <c r="C13" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -1451,7 +1432,7 @@
         <v>68</v>
       </c>
       <c r="C14" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -1462,7 +1443,7 @@
         <v>69</v>
       </c>
       <c r="C15" t="s">
-        <v>136</v>
+        <v>154</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -1473,7 +1454,7 @@
         <v>65</v>
       </c>
       <c r="C16" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -1484,7 +1465,7 @@
         <v>64</v>
       </c>
       <c r="C17" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1495,7 +1476,7 @@
         <v>66</v>
       </c>
       <c r="C18" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -1506,7 +1487,7 @@
         <v>78</v>
       </c>
       <c r="C19" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -1517,7 +1498,7 @@
         <v>79</v>
       </c>
       <c r="C20" t="s">
-        <v>141</v>
+        <v>124</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -1528,7 +1509,7 @@
         <v>80</v>
       </c>
       <c r="C21" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -1539,7 +1520,7 @@
         <v>81</v>
       </c>
       <c r="C22" t="s">
-        <v>143</v>
+        <v>128</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -1550,7 +1531,7 @@
         <v>82</v>
       </c>
       <c r="C23" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -1561,7 +1542,7 @@
         <v>83</v>
       </c>
       <c r="C24" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -1572,7 +1553,7 @@
         <v>84</v>
       </c>
       <c r="C25" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -1583,7 +1564,7 @@
         <v>85</v>
       </c>
       <c r="C26" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -1594,7 +1575,7 @@
         <v>86</v>
       </c>
       <c r="C27" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -1605,7 +1586,7 @@
         <v>87</v>
       </c>
       <c r="C28" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -1616,7 +1597,7 @@
         <v>88</v>
       </c>
       <c r="C29" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -1627,7 +1608,7 @@
         <v>89</v>
       </c>
       <c r="C30" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -1638,7 +1619,7 @@
         <v>90</v>
       </c>
       <c r="C31" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -1649,7 +1630,7 @@
         <v>91</v>
       </c>
       <c r="C32" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -1660,7 +1641,7 @@
         <v>92</v>
       </c>
       <c r="C33" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -1913,7 +1894,7 @@
         <v>115</v>
       </c>
       <c r="C56" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -1924,7 +1905,7 @@
         <v>116</v>
       </c>
       <c r="C57" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -1935,7 +1916,7 @@
         <v>117</v>
       </c>
       <c r="C58" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -2155,31 +2136,6 @@
     <row r="97" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C97" t="s">
         <v>210</v>
-      </c>
-    </row>
-    <row r="98" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C98" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="99" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C99" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="100" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C100" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="101" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C101" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="102" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C102" t="s">
-        <v>215</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed UG Health and GI bugs
</commit_message>
<xml_diff>
--- a/App/uap_cross_sell/www/files/cs_upload_template.xlsx
+++ b/App/uap_cross_sell/www/files/cs_upload_template.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Contracts\UAP\D - Working Papers\UAP-cross-sell\App\uap_cross_sell\www\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tayojabar/Documents/OML/UAP-cross-sell/UAP-cross-sell/App/uap_cross_sell/www/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2B17867-B4A3-45FB-A13E-5888156D3F81}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48D50902-7EB5-8B42-8E12-111EA1BBABA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{24700C77-9C92-4468-B9C5-B77420552ACF}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{24700C77-9C92-4468-B9C5-B77420552ACF}"/>
   </bookViews>
   <sheets>
     <sheet name="customer_acc" sheetId="1" r:id="rId1"/>
     <sheet name="customer_prod" sheetId="2" r:id="rId2"/>
-    <sheet name="valid_product_names" sheetId="3" state="hidden" r:id="rId3"/>
+    <sheet name="valid_product_names" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="Kenya">valid_product_names!$A$2:$A$62</definedName>
-    <definedName name="Uganda">valid_product_names!$C$2:$C$97</definedName>
+    <definedName name="Nigeria">valid_product_names!$D$2:$D$54</definedName>
+    <definedName name="Uganda">valid_product_names!$C$2:$C$51</definedName>
     <definedName name="Zimbabwe">valid_product_names!$B$2:$B$62</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="218">
   <si>
     <t>Old Mutual Equity Fund</t>
   </si>
@@ -403,180 +404,6 @@
     <t>Uganda</t>
   </si>
   <si>
-    <t>CHRONIC / HIV-AIDS / PRE-EXISTING DISEASE</t>
-  </si>
-  <si>
-    <t>CHRONIC / PRE-EXISTING / HIV / CANCER</t>
-  </si>
-  <si>
-    <t>CONGENITAL DISEASE</t>
-  </si>
-  <si>
-    <t>DENTAL</t>
-  </si>
-  <si>
-    <t>DENTAL BRIDGES</t>
-  </si>
-  <si>
-    <t>DENTAL CROWNS</t>
-  </si>
-  <si>
-    <t>DENTAL DENTURES</t>
-  </si>
-  <si>
-    <t>DENTAL SURGERY</t>
-  </si>
-  <si>
-    <t>FUNERAL</t>
-  </si>
-  <si>
-    <t>GYNAECOLOGICAL SURGERY</t>
-  </si>
-  <si>
-    <t>ILLNESS</t>
-  </si>
-  <si>
-    <t>IN-PATIENT</t>
-  </si>
-  <si>
-    <t>LODGER`S FEE</t>
-  </si>
-  <si>
-    <t>MATERNITY</t>
-  </si>
-  <si>
-    <t>MATERNITY / CAESAREAN</t>
-  </si>
-  <si>
-    <t>MAXILLOFACIAL AND ORAL SURGERY</t>
-  </si>
-  <si>
-    <t>OPTHALMOLOGY</t>
-  </si>
-  <si>
-    <t>OPTICAL</t>
-  </si>
-  <si>
-    <t>ORGAN TRANSPLANT</t>
-  </si>
-  <si>
-    <t>OUT-PATIENT</t>
-  </si>
-  <si>
-    <t>PROSTHESIS APPLIANCES</t>
-  </si>
-  <si>
-    <t>PSYCHIATRIC / PHYSIOTHERAPY</t>
-  </si>
-  <si>
-    <t>PSYCHIATRIC TREATMENT</t>
-  </si>
-  <si>
-    <t>RECONSTRUCTIVE SURGERY</t>
-  </si>
-  <si>
-    <t>ROOM CHARGE DAY LIMIT</t>
-  </si>
-  <si>
-    <t>VISIT FEE</t>
-  </si>
-  <si>
-    <t>ANNUAL MEDICAL CHECK-UP</t>
-  </si>
-  <si>
-    <t>CHRONIC / PRE-EXISTING / HIV / MATERNITY</t>
-  </si>
-  <si>
-    <t>CONGENITAL AND NEONATAL CONDITION</t>
-  </si>
-  <si>
-    <t>CANCER TREATMENT</t>
-  </si>
-  <si>
-    <t>IMMUNIZATION</t>
-  </si>
-  <si>
-    <t>POST-HOSPITALIZATION</t>
-  </si>
-  <si>
-    <t>MATERNITY / EMERGENCY CAESAREAN</t>
-  </si>
-  <si>
-    <t>NEONATAL</t>
-  </si>
-  <si>
-    <t>MATERNITY (CAESAREAN)</t>
-  </si>
-  <si>
-    <t>SPECTACLE FRAME</t>
-  </si>
-  <si>
-    <t>HIV / AIDS</t>
-  </si>
-  <si>
-    <t>ROOM CHARGE</t>
-  </si>
-  <si>
-    <t>CHRONIC / CONGENITAL</t>
-  </si>
-  <si>
-    <t>ANNUAL MEDICAL CHECK-UP FOR MAIN MEMBER / EMPLOYEE</t>
-  </si>
-  <si>
-    <t>EXCESS OF LOSS</t>
-  </si>
-  <si>
-    <t>ANNUAL MEDICAL CHECK-UP FOR DEPANDANT</t>
-  </si>
-  <si>
-    <t>CONTACT LENSES</t>
-  </si>
-  <si>
-    <t>DENTAL CLEANING</t>
-  </si>
-  <si>
-    <t>DENTAL EXTRACTIONS</t>
-  </si>
-  <si>
-    <t>DENTAL FILLING</t>
-  </si>
-  <si>
-    <t>DENTAL POLISHING</t>
-  </si>
-  <si>
-    <t>DENTAL ROOT CANAL</t>
-  </si>
-  <si>
-    <t>DENTAL SCALING</t>
-  </si>
-  <si>
-    <t>EYE TEST</t>
-  </si>
-  <si>
-    <t>VACCINATION</t>
-  </si>
-  <si>
-    <t>MATERNITY RELATED AILMENT</t>
-  </si>
-  <si>
-    <t>PHYSIOTHERAPY</t>
-  </si>
-  <si>
-    <t>PERSONAL ACCIDENT</t>
-  </si>
-  <si>
-    <t>MATERNITY / MATERNITY RELATED AILMENT</t>
-  </si>
-  <si>
-    <t>ANTENATAL AND POSTNATAL COVER</t>
-  </si>
-  <si>
-    <t>MEDICAL AIDS</t>
-  </si>
-  <si>
-    <t>CHRONIC / PRE-EXISTING / CONGENITAL</t>
-  </si>
-  <si>
     <t>FIRE COMMERCIAL</t>
   </si>
   <si>
@@ -680,13 +507,193 @@
   </si>
   <si>
     <t>Structured Order Finance Loan</t>
+  </si>
+  <si>
+    <t>SERENICARE INDIVIDUAL AND FAMILY COVER</t>
+  </si>
+  <si>
+    <t>SERENICARE</t>
+  </si>
+  <si>
+    <t>RETAIL</t>
+  </si>
+  <si>
+    <t>L.O.P. FOLLOWING MACHINERY B/DOWN</t>
+  </si>
+  <si>
+    <t>RETENTION BOND</t>
+  </si>
+  <si>
+    <t>AVIATION</t>
+  </si>
+  <si>
+    <t>LIVESTOCK</t>
+  </si>
+  <si>
+    <t>MOTOR THIRD PARTY OUTLET</t>
+  </si>
+  <si>
+    <t>CROP INSURANCE - AGRIC CONSORTIUM</t>
+  </si>
+  <si>
+    <t>FTB CARE GIVER</t>
+  </si>
+  <si>
+    <t>Nigeria</t>
+  </si>
+  <si>
+    <t>Savings Product</t>
+  </si>
+  <si>
+    <t>Family Risk Product</t>
+  </si>
+  <si>
+    <t>Life Product</t>
+  </si>
+  <si>
+    <t>GROUP LIFE ONLY</t>
+  </si>
+  <si>
+    <t>CREDIT LIFE ASSURANCE</t>
+  </si>
+  <si>
+    <t>INVESTMENT LINK SCHEME</t>
+  </si>
+  <si>
+    <t>OCEANIC EDUCATION ASSURANCE POLICY</t>
+  </si>
+  <si>
+    <t>OCEANFLEX CONTRIBUTION ASS. SCHEME</t>
+  </si>
+  <si>
+    <t>OCEANTAP</t>
+  </si>
+  <si>
+    <t>OCEANIC EDUCATION ASSURANCE POLICY1</t>
+  </si>
+  <si>
+    <t>CREDIT LIFE ASSURANCE 2</t>
+  </si>
+  <si>
+    <t>TERM ASSURANCE</t>
+  </si>
+  <si>
+    <t>TERM ASS. WITH REFUND</t>
+  </si>
+  <si>
+    <t>MORTGAGE PROTECTION SCHEME</t>
+  </si>
+  <si>
+    <t>OCEANIC BABY PLAN</t>
+  </si>
+  <si>
+    <t>NATA</t>
+  </si>
+  <si>
+    <t>Public Liability (not energy Risks)</t>
+  </si>
+  <si>
+    <t>Specified Cars</t>
+  </si>
+  <si>
+    <t>Fire and Perils</t>
+  </si>
+  <si>
+    <t>Plant All Risks</t>
+  </si>
+  <si>
+    <t>Householders</t>
+  </si>
+  <si>
+    <t>Specified Commercial Vehicles</t>
+  </si>
+  <si>
+    <t>Cargo</t>
+  </si>
+  <si>
+    <t>Industrial All Risks</t>
+  </si>
+  <si>
+    <t>Co-Insurance</t>
+  </si>
+  <si>
+    <t>Contractor All Risk (not energy Risks)</t>
+  </si>
+  <si>
+    <t>Employer's Liability</t>
+  </si>
+  <si>
+    <t>Advance Payment Bonds</t>
+  </si>
+  <si>
+    <t>All Risks</t>
+  </si>
+  <si>
+    <t>Burglary</t>
+  </si>
+  <si>
+    <t>Group Personal Accident</t>
+  </si>
+  <si>
+    <t>Hull</t>
+  </si>
+  <si>
+    <t>Workmen's Compensation</t>
+  </si>
+  <si>
+    <t>Energy Exploration/Development</t>
+  </si>
+  <si>
+    <t>Specified Motorcycles</t>
+  </si>
+  <si>
+    <t>Specified Trailers &amp; Cars</t>
+  </si>
+  <si>
+    <t>Consequential Loss</t>
+  </si>
+  <si>
+    <t>Fidelity</t>
+  </si>
+  <si>
+    <t>Goods in transit</t>
+  </si>
+  <si>
+    <t>Boiler/Pressure Vessels</t>
+  </si>
+  <si>
+    <t>Electronic Equipment</t>
+  </si>
+  <si>
+    <t>Combined Fire and Theft</t>
+  </si>
+  <si>
+    <t>Money</t>
+  </si>
+  <si>
+    <t>Specified Trailers &amp; Comm veh</t>
+  </si>
+  <si>
+    <t>Aviation Hull</t>
+  </si>
+  <si>
+    <t>Director or Officers</t>
+  </si>
+  <si>
+    <t>Performance/Construction Bonds</t>
+  </si>
+  <si>
+    <t>Erection All Risks (not energy Risks)</t>
+  </si>
+  <si>
+    <t>Counter Guarantee</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -709,6 +716,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -752,11 +765,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1074,83 +1088,87 @@
   <dimension ref="A1:A19"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1537</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>1418</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>100003</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>101403</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>1016908</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>1024783</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>1016764</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>1023406</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
     </row>
   </sheetData>
@@ -1163,17 +1181,17 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="34.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
@@ -1181,67 +1199,65 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>125</v>
+        <v>26</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="2"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
     </row>
   </sheetData>
@@ -1256,7 +1272,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F06FDF89-FCC4-438E-B054-39500F380DC7}">
           <x14:formula1>
-            <xm:f>valid_product_names!$A$1:$C$1</xm:f>
+            <xm:f>valid_product_names!$A$1:$D$1</xm:f>
           </x14:formula1>
           <xm:sqref>C2</xm:sqref>
         </x14:dataValidation>
@@ -1268,20 +1284,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35D5C44B-F88A-4340-B982-5E1C9A94327D}">
-  <dimension ref="A1:C97"/>
+  <dimension ref="A1:D62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" activeCellId="2" sqref="A1:A62 B1:B62 C1:C97"/>
+      <selection activeCell="D1" activeCellId="3" sqref="A1:A62 B1:B62 C1:C51 D1:D54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="37" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="54.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="56.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="56.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>63</v>
       </c>
@@ -1291,851 +1307,805 @@
       <c r="C1" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>67</v>
       </c>
-      <c r="C2" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C2" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="D2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>211</v>
-      </c>
-      <c r="C3" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" t="s">
         <v>74</v>
       </c>
-      <c r="C4" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C4" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="D4" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
       <c r="B5" t="s">
         <v>75</v>
       </c>
-      <c r="C5" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C5" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="D5" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>1</v>
       </c>
       <c r="B6" t="s">
         <v>76</v>
       </c>
-      <c r="C6" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>212</v>
-      </c>
-      <c r="C7" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>213</v>
-      </c>
-      <c r="C8" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="D8" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>214</v>
-      </c>
-      <c r="C9" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="D9" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>215</v>
-      </c>
-      <c r="C10" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>11</v>
       </c>
       <c r="B11" t="s">
         <v>77</v>
       </c>
-      <c r="C11" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C11" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="D11" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
       <c r="B12" t="s">
         <v>71</v>
       </c>
-      <c r="C12" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C12" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D12" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>13</v>
       </c>
       <c r="B13" t="s">
         <v>70</v>
       </c>
-      <c r="C13" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C13" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="D13" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>14</v>
       </c>
       <c r="B14" t="s">
         <v>68</v>
       </c>
-      <c r="C14" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C14" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="D14" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>15</v>
       </c>
       <c r="B15" t="s">
         <v>69</v>
       </c>
-      <c r="C15" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C15" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="D15" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>16</v>
       </c>
       <c r="B16" t="s">
         <v>65</v>
       </c>
-      <c r="C16" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C16" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="D16" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>17</v>
       </c>
       <c r="B17" t="s">
         <v>64</v>
       </c>
-      <c r="C17" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C17" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>18</v>
       </c>
       <c r="B18" t="s">
         <v>66</v>
       </c>
-      <c r="C18" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C18" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>19</v>
       </c>
       <c r="B19" t="s">
         <v>78</v>
       </c>
-      <c r="C19" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C19" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="D19" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>20</v>
       </c>
       <c r="B20" t="s">
         <v>79</v>
       </c>
-      <c r="C20" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C20" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="D20" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>21</v>
       </c>
       <c r="B21" t="s">
         <v>80</v>
       </c>
-      <c r="C21" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C21" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="D21" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>22</v>
       </c>
       <c r="B22" t="s">
         <v>81</v>
       </c>
-      <c r="C22" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C22" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="D22" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>23</v>
       </c>
       <c r="B23" t="s">
         <v>82</v>
       </c>
-      <c r="C23" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C23" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="D23" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>24</v>
       </c>
       <c r="B24" t="s">
         <v>83</v>
       </c>
-      <c r="C24" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C24" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="D24" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>25</v>
       </c>
       <c r="B25" t="s">
         <v>84</v>
       </c>
-      <c r="C25" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C25" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="D25" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>26</v>
       </c>
       <c r="B26" t="s">
         <v>85</v>
       </c>
-      <c r="C26" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C26" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>27</v>
       </c>
       <c r="B27" t="s">
         <v>86</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>28</v>
       </c>
       <c r="B28" t="s">
         <v>87</v>
       </c>
-      <c r="C28" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C28" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="D28" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>29</v>
       </c>
       <c r="B29" t="s">
         <v>88</v>
       </c>
-      <c r="C29" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C29" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D29" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>30</v>
       </c>
       <c r="B30" t="s">
         <v>89</v>
       </c>
-      <c r="C30" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C30" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D30" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>31</v>
       </c>
       <c r="B31" t="s">
         <v>90</v>
       </c>
-      <c r="C31" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C31" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D31" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>32</v>
       </c>
       <c r="B32" t="s">
         <v>91</v>
       </c>
-      <c r="C32" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C32" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="D32" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>33</v>
       </c>
       <c r="B33" t="s">
         <v>92</v>
       </c>
-      <c r="C33" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C33" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="D33" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>34</v>
       </c>
       <c r="B34" t="s">
         <v>93</v>
       </c>
-      <c r="C34" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C34" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="D34" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>35</v>
       </c>
       <c r="B35" t="s">
         <v>94</v>
       </c>
-      <c r="C35" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C35" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="D35" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>36</v>
       </c>
       <c r="B36" t="s">
         <v>95</v>
       </c>
-      <c r="C36" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C36" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="D36" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>37</v>
       </c>
       <c r="B37" t="s">
         <v>96</v>
       </c>
-      <c r="C37" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C37" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="D37" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>38</v>
       </c>
       <c r="B38" t="s">
         <v>97</v>
       </c>
-      <c r="C38" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C38" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="D38" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>39</v>
       </c>
       <c r="B39" t="s">
         <v>98</v>
       </c>
-      <c r="C39" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C39" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="D39" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>40</v>
       </c>
       <c r="B40" t="s">
         <v>99</v>
       </c>
-      <c r="C40" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C40" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="D40" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>41</v>
       </c>
       <c r="B41" t="s">
         <v>100</v>
       </c>
-      <c r="C41" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C41" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="D41" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>42</v>
       </c>
       <c r="B42" t="s">
         <v>101</v>
       </c>
-      <c r="C42" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C42" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="D42" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>43</v>
       </c>
       <c r="B43" t="s">
         <v>102</v>
       </c>
-      <c r="C43" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C43" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="D43" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>44</v>
       </c>
       <c r="B44" t="s">
         <v>103</v>
       </c>
-      <c r="C44" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C44" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="D44" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>45</v>
       </c>
       <c r="B45" t="s">
         <v>104</v>
       </c>
-      <c r="C45" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C45" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="D45" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>46</v>
       </c>
       <c r="B46" t="s">
         <v>105</v>
       </c>
-      <c r="C46" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C46" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="D46" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>47</v>
       </c>
       <c r="B47" t="s">
         <v>106</v>
       </c>
-      <c r="C47" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C47" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D47" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>48</v>
       </c>
       <c r="B48" t="s">
         <v>107</v>
       </c>
-      <c r="C48" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C48" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="D48" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>49</v>
       </c>
       <c r="B49" t="s">
         <v>108</v>
       </c>
-      <c r="C49" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C49" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="D49" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>50</v>
       </c>
       <c r="B50" t="s">
         <v>109</v>
       </c>
-      <c r="C50" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C50" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="D50" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>51</v>
       </c>
       <c r="B51" t="s">
         <v>110</v>
       </c>
-      <c r="C51" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C51" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="D51" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>52</v>
       </c>
       <c r="B52" t="s">
         <v>111</v>
       </c>
-      <c r="C52" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D52" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>53</v>
       </c>
       <c r="B53" t="s">
         <v>112</v>
       </c>
-      <c r="C53" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D53" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>54</v>
       </c>
       <c r="B54" t="s">
         <v>113</v>
       </c>
-      <c r="C54" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D54" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>55</v>
       </c>
       <c r="B55" t="s">
         <v>114</v>
       </c>
-      <c r="C55" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>56</v>
       </c>
       <c r="B56" t="s">
         <v>115</v>
       </c>
-      <c r="C56" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>57</v>
       </c>
       <c r="B57" t="s">
         <v>116</v>
       </c>
-      <c r="C57" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>58</v>
       </c>
       <c r="B58" t="s">
         <v>117</v>
       </c>
-      <c r="C58" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>59</v>
       </c>
       <c r="B59" t="s">
         <v>118</v>
       </c>
-      <c r="C59" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>60</v>
       </c>
       <c r="B60" t="s">
         <v>119</v>
       </c>
-      <c r="C60" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>61</v>
       </c>
       <c r="B61" t="s">
         <v>120</v>
       </c>
-      <c r="C61" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>62</v>
       </c>
       <c r="B62" t="s">
         <v>121</v>
-      </c>
-      <c r="C62" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C63" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C64" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="65" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C65" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="66" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C66" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="67" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C67" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="68" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C68" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="69" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C69" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="70" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C70" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="71" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C71" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="72" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C72" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="73" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C73" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="74" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C74" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="75" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C75" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="76" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C76" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="77" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C77" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="78" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C78" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="79" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C79" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="80" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C80" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="81" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C81" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="82" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C82" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="83" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C83" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="84" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C84" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="85" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C85" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="86" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C86" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="87" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C87" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="88" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C88" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="89" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C89" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="90" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C90" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="91" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C91" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="92" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C92" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="93" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C93" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="94" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C94" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="95" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C95" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="96" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C96" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="97" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C97" t="s">
-        <v>210</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Hid the valid_products worksheet
</commit_message>
<xml_diff>
--- a/App/uap_cross_sell/www/files/cs_upload_template.xlsx
+++ b/App/uap_cross_sell/www/files/cs_upload_template.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tayojabar/Documents/OML/UAP-cross-sell/UAP-cross-sell/App/uap_cross_sell/www/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Contracts\UAP\D - Working Papers\UAP-cross-sell\App\uap_cross_sell\www\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48D50902-7EB5-8B42-8E12-111EA1BBABA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11BBA2E7-E3AF-404C-BD0B-0BF770E48942}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{24700C77-9C92-4468-B9C5-B77420552ACF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{24700C77-9C92-4468-B9C5-B77420552ACF}"/>
   </bookViews>
   <sheets>
     <sheet name="customer_acc" sheetId="1" r:id="rId1"/>
     <sheet name="customer_prod" sheetId="2" r:id="rId2"/>
-    <sheet name="valid_product_names" sheetId="3" r:id="rId3"/>
+    <sheet name="valid_product_names" sheetId="3" state="hidden" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="Kenya">valid_product_names!$A$2:$A$62</definedName>
@@ -693,7 +693,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1087,88 +1087,88 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C783F41-9AF8-4698-A4E2-A0CDF8EF2C34}">
   <dimension ref="A1:A19"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" s="1" customFormat="1">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1">
       <c r="A2" s="2">
         <v>1537</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1">
       <c r="A3" s="2">
         <v>1418</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1">
       <c r="A4" s="2">
         <v>100003</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1">
       <c r="A5" s="2">
         <v>101403</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1">
       <c r="A6" s="2">
         <v>1016908</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:1">
       <c r="A7" s="2">
         <v>1024783</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:1">
       <c r="A8" s="2">
         <v>1016764</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:1">
       <c r="A9" s="2">
         <v>1023406</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:1">
       <c r="A10" s="2"/>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:1">
       <c r="A11" s="2"/>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:1">
       <c r="A12" s="2"/>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:1">
       <c r="A13" s="2"/>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:1">
       <c r="A14" s="2"/>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:1">
       <c r="A15" s="2"/>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:1">
       <c r="A16" s="2"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1">
       <c r="A17" s="2"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1">
       <c r="A18" s="2"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1">
       <c r="A19" s="2"/>
     </row>
   </sheetData>
@@ -1180,18 +1180,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A24E3401-6C35-4108-BA35-AB6F39FFE1F7}">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="34.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" s="1" customFormat="1">
       <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
@@ -1199,7 +1199,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
         <v>26</v>
       </c>
@@ -1207,57 +1207,57 @@
         <v>168</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4" s="2"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="A5" s="2"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3">
       <c r="A6" s="2"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3">
       <c r="A7" s="2"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3">
       <c r="A8" s="2"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3">
       <c r="A9" s="2"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3">
       <c r="A10" s="2"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3">
       <c r="A11" s="2"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3">
       <c r="A12" s="2"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3">
       <c r="A13" s="2"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3">
       <c r="A14" s="2"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3">
       <c r="A15" s="2"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3">
       <c r="A16" s="2"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1">
       <c r="A17" s="2"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1">
       <c r="A18" s="2"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1">
       <c r="A19" s="2"/>
     </row>
   </sheetData>
@@ -1290,14 +1290,14 @@
       <selection activeCell="D1" activeCellId="3" sqref="A1:A62 B1:B62 C1:C51 D1:D54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="37" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="54.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="56.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="56.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>63</v>
       </c>
@@ -1311,7 +1311,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1325,7 +1325,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1339,7 +1339,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1353,7 +1353,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1367,7 +1367,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -1381,7 +1381,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -1395,7 +1395,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -1409,7 +1409,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1423,7 +1423,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -1437,7 +1437,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1451,7 +1451,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1465,7 +1465,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1479,7 +1479,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1493,7 +1493,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -1507,7 +1507,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -1521,7 +1521,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -1535,7 +1535,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -1549,7 +1549,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -1563,7 +1563,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -1577,7 +1577,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -1591,7 +1591,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -1605,7 +1605,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -1619,7 +1619,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -1633,7 +1633,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -1647,7 +1647,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -1661,7 +1661,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -1675,7 +1675,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -1689,7 +1689,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -1703,7 +1703,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -1717,7 +1717,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -1731,7 +1731,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4">
       <c r="A32" t="s">
         <v>32</v>
       </c>
@@ -1745,7 +1745,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4">
       <c r="A33" t="s">
         <v>33</v>
       </c>
@@ -1759,7 +1759,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4">
       <c r="A34" t="s">
         <v>34</v>
       </c>
@@ -1773,7 +1773,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4">
       <c r="A35" t="s">
         <v>35</v>
       </c>
@@ -1787,7 +1787,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -1801,7 +1801,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4">
       <c r="A37" t="s">
         <v>37</v>
       </c>
@@ -1815,7 +1815,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4">
       <c r="A38" t="s">
         <v>38</v>
       </c>
@@ -1829,7 +1829,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4">
       <c r="A39" t="s">
         <v>39</v>
       </c>
@@ -1843,7 +1843,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4">
       <c r="A40" t="s">
         <v>40</v>
       </c>
@@ -1857,7 +1857,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4">
       <c r="A41" t="s">
         <v>41</v>
       </c>
@@ -1871,7 +1871,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4">
       <c r="A42" t="s">
         <v>42</v>
       </c>
@@ -1885,7 +1885,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4">
       <c r="A43" t="s">
         <v>43</v>
       </c>
@@ -1899,7 +1899,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4">
       <c r="A44" t="s">
         <v>44</v>
       </c>
@@ -1913,7 +1913,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4">
       <c r="A45" t="s">
         <v>45</v>
       </c>
@@ -1927,7 +1927,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4">
       <c r="A46" t="s">
         <v>46</v>
       </c>
@@ -1941,7 +1941,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4">
       <c r="A47" t="s">
         <v>47</v>
       </c>
@@ -1955,7 +1955,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4">
       <c r="A48" t="s">
         <v>48</v>
       </c>
@@ -1969,7 +1969,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4">
       <c r="A49" t="s">
         <v>49</v>
       </c>
@@ -1983,7 +1983,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4">
       <c r="A50" t="s">
         <v>50</v>
       </c>
@@ -1997,7 +1997,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4">
       <c r="A51" t="s">
         <v>51</v>
       </c>
@@ -2011,7 +2011,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4">
       <c r="A52" t="s">
         <v>52</v>
       </c>
@@ -2022,7 +2022,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4">
       <c r="A53" t="s">
         <v>53</v>
       </c>
@@ -2033,7 +2033,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4">
       <c r="A54" t="s">
         <v>54</v>
       </c>
@@ -2044,7 +2044,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4">
       <c r="A55" t="s">
         <v>55</v>
       </c>
@@ -2052,7 +2052,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4">
       <c r="A56" t="s">
         <v>56</v>
       </c>
@@ -2060,7 +2060,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4">
       <c r="A57" t="s">
         <v>57</v>
       </c>
@@ -2068,7 +2068,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4">
       <c r="A58" t="s">
         <v>58</v>
       </c>
@@ -2076,7 +2076,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4">
       <c r="A59" t="s">
         <v>59</v>
       </c>
@@ -2084,7 +2084,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4">
       <c r="A60" t="s">
         <v>60</v>
       </c>
@@ -2092,7 +2092,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4">
       <c r="A61" t="s">
         <v>61</v>
       </c>
@@ -2100,7 +2100,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4">
       <c r="A62" t="s">
         <v>62</v>
       </c>

</xml_diff>

<commit_message>
GH Cross-sell for Life
</commit_message>
<xml_diff>
--- a/App/uap_cross_sell/www/files/cs_upload_template.xlsx
+++ b/App/uap_cross_sell/www/files/cs_upload_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tayojabar/Documents/OML/UAP-cross-sell/UAP-cross-sell/App/uap_cross_sell/www/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48D50902-7EB5-8B42-8E12-111EA1BBABA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE4AE1CC-D5E9-4F43-A84C-30DF25AA8578}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{24700C77-9C92-4468-B9C5-B77420552ACF}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{24700C77-9C92-4468-B9C5-B77420552ACF}"/>
   </bookViews>
   <sheets>
     <sheet name="customer_acc" sheetId="1" r:id="rId1"/>
@@ -18,10 +18,11 @@
     <sheet name="valid_product_names" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="Kenya">valid_product_names!$A$2:$A$62</definedName>
+    <definedName name="Ghana">valid_product_names!$E$2:$E$16</definedName>
+    <definedName name="Kenya">valid_product_names!$A$2:$A$54</definedName>
     <definedName name="Nigeria">valid_product_names!$D$2:$D$54</definedName>
-    <definedName name="Uganda">valid_product_names!$C$2:$C$51</definedName>
-    <definedName name="Zimbabwe">valid_product_names!$B$2:$B$62</definedName>
+    <definedName name="Uganda">valid_product_names!$C$2:$C$54</definedName>
+    <definedName name="Zimbabwe">valid_product_names!$B$2:$B$54</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="236">
   <si>
     <t>Old Mutual Equity Fund</t>
   </si>
@@ -687,6 +688,60 @@
   </si>
   <si>
     <t>Counter Guarantee</t>
+  </si>
+  <si>
+    <t>Ghana</t>
+  </si>
+  <si>
+    <t>PRODUCTS</t>
+  </si>
+  <si>
+    <t>INTERNATIONAL TRAVEL</t>
+  </si>
+  <si>
+    <t>50 PLUS SECURITY PLAN</t>
+  </si>
+  <si>
+    <t>EDUCATOR PLAN</t>
+  </si>
+  <si>
+    <t>PERSONAL ACCIDENT</t>
+  </si>
+  <si>
+    <t>SPECIAL INVESTMENT PLAN</t>
+  </si>
+  <si>
+    <t>FUNERAL EXPENSES POLICY</t>
+  </si>
+  <si>
+    <t>MORTGAGE PROTECTION</t>
+  </si>
+  <si>
+    <t>TRANSITION PLAN (FUNERAL POLICY)</t>
+  </si>
+  <si>
+    <t>TRANSITION (FUNERAL) PLAN</t>
+  </si>
+  <si>
+    <t>ECOBANK RETIREMENT SAVINGS PLAN</t>
+  </si>
+  <si>
+    <t>TERM ASSURANCE POLICY</t>
+  </si>
+  <si>
+    <t>WELFARE PLAN</t>
+  </si>
+  <si>
+    <t>TRANSITION PLAN (BANCASSURANCE)</t>
+  </si>
+  <si>
+    <t>TRANSITION PLUS PLAN - RETAIL</t>
+  </si>
+  <si>
+    <t>AG002068</t>
+  </si>
+  <si>
+    <t>AS000883</t>
   </si>
 </sst>
 </file>
@@ -765,12 +820,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1087,89 +1145,93 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C783F41-9AF8-4698-A4E2-A0CDF8EF2C34}">
   <dimension ref="A1:A19"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.5" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2">
+      <c r="A2" s="6">
         <v>1537</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2">
+      <c r="A3" s="6">
         <v>1418</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
+      <c r="A4" s="6">
         <v>100003</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
+      <c r="A5" s="6">
         <v>101403</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="2">
+      <c r="A6" s="6">
         <v>1016908</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" s="2">
+      <c r="A7" s="6">
         <v>1024783</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" s="2">
+      <c r="A8" s="6">
         <v>1016764</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" s="2">
+      <c r="A9" s="6">
         <v>1023406</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" s="2"/>
+      <c r="A10" s="6" t="s">
+        <v>234</v>
+      </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" s="2"/>
+      <c r="A11" s="6" t="s">
+        <v>235</v>
+      </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" s="2"/>
+      <c r="A12" s="6"/>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" s="2"/>
+      <c r="A13" s="6"/>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A14" s="2"/>
+      <c r="A14" s="6"/>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A15" s="2"/>
+      <c r="A15" s="6"/>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A16" s="2"/>
+      <c r="A16" s="6"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="2"/>
+      <c r="A17" s="6"/>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="2"/>
+      <c r="A18" s="6"/>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="2"/>
+      <c r="A19" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1180,8 +1242,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A24E3401-6C35-4108-BA35-AB6F39FFE1F7}">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1201,10 +1263,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>26</v>
+        <v>225</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>168</v>
+        <v>218</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1272,7 +1334,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F06FDF89-FCC4-438E-B054-39500F380DC7}">
           <x14:formula1>
-            <xm:f>valid_product_names!$A$1:$D$1</xm:f>
+            <xm:f>valid_product_names!$A$1:$E$1</xm:f>
           </x14:formula1>
           <xm:sqref>C2</xm:sqref>
         </x14:dataValidation>
@@ -1284,10 +1346,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35D5C44B-F88A-4340-B982-5E1C9A94327D}">
-  <dimension ref="A1:D62"/>
+  <dimension ref="A1:E62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" activeCellId="3" sqref="A1:A62 B1:B62 C1:C51 D1:D54"/>
+      <selection activeCell="E1" activeCellId="4" sqref="A1:A62 B1:B62 C1:C51 A1:D54 E1:E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1295,9 +1357,10 @@
     <col min="1" max="1" width="37" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="54.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="56.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>63</v>
       </c>
@@ -1310,8 +1373,11 @@
       <c r="D1" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1324,8 +1390,11 @@
       <c r="D2" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1338,8 +1407,11 @@
       <c r="D3" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1352,8 +1424,11 @@
       <c r="D4" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1366,8 +1441,11 @@
       <c r="D5" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -1380,8 +1458,11 @@
       <c r="D6" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E6" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -1394,8 +1475,11 @@
       <c r="D7" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E7" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -1408,8 +1492,11 @@
       <c r="D8" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E8" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1422,8 +1509,11 @@
       <c r="D9" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E9" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -1436,8 +1526,11 @@
       <c r="D10" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E10" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1450,8 +1543,11 @@
       <c r="D11" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E11" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1464,8 +1560,11 @@
       <c r="D12" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E12" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1478,8 +1577,11 @@
       <c r="D13" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E13" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1492,8 +1594,11 @@
       <c r="D14" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E14" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -1506,8 +1611,11 @@
       <c r="D15" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E15" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -1519,6 +1627,9 @@
       </c>
       <c r="D16" t="s">
         <v>183</v>
+      </c>
+      <c r="E16" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
General Insurance cross-sell Sudan
</commit_message>
<xml_diff>
--- a/App/uap_cross_sell/www/files/cs_upload_template.xlsx
+++ b/App/uap_cross_sell/www/files/cs_upload_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tayojabar/Documents/OML/UAP-cross-sell/UAP-cross-sell/App/uap_cross_sell/www/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE4AE1CC-D5E9-4F43-A84C-30DF25AA8578}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FAE6ECC-8ECE-1140-AC59-DB84DDB02184}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{24700C77-9C92-4468-B9C5-B77420552ACF}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16440" xr2:uid="{24700C77-9C92-4468-B9C5-B77420552ACF}"/>
   </bookViews>
   <sheets>
     <sheet name="customer_acc" sheetId="1" r:id="rId1"/>
@@ -19,10 +19,11 @@
   </sheets>
   <definedNames>
     <definedName name="Ghana">valid_product_names!$E$2:$E$16</definedName>
-    <definedName name="Kenya">valid_product_names!$A$2:$A$54</definedName>
+    <definedName name="Kenya">valid_product_names!$A$2:$A$62</definedName>
     <definedName name="Nigeria">valid_product_names!$D$2:$D$54</definedName>
-    <definedName name="Uganda">valid_product_names!$C$2:$C$54</definedName>
-    <definedName name="Zimbabwe">valid_product_names!$B$2:$B$54</definedName>
+    <definedName name="Sudan">valid_product_names!$F$2:$F$35</definedName>
+    <definedName name="Uganda">valid_product_names!$C$2:$C$51</definedName>
+    <definedName name="Zimbabwe">valid_product_names!$B$2:$B$62</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="254">
   <si>
     <t>Old Mutual Equity Fund</t>
   </si>
@@ -742,6 +743,60 @@
   </si>
   <si>
     <t>AS000883</t>
+  </si>
+  <si>
+    <t>Sudan</t>
+  </si>
+  <si>
+    <t>TRUCKSURE</t>
+  </si>
+  <si>
+    <t>MOTORSURE</t>
+  </si>
+  <si>
+    <t>GROUP PERSONAL ACCIDENT</t>
+  </si>
+  <si>
+    <t>HEALTH/MEDICAL EXPENSES INSURANCE</t>
+  </si>
+  <si>
+    <t>WORKMEN'S COMP (COMMON LAW) COVER</t>
+  </si>
+  <si>
+    <t>MOTOR P.T.A. COVER</t>
+  </si>
+  <si>
+    <t>MOTOR TRACTORS</t>
+  </si>
+  <si>
+    <t>OFFICE COMPACT</t>
+  </si>
+  <si>
+    <t>MOTOR (PSV) PRIVATE HIRE</t>
+  </si>
+  <si>
+    <t>PERFORMANCE BONDS</t>
+  </si>
+  <si>
+    <t>HEALTH/MEDICAL - OUTPATIENT</t>
+  </si>
+  <si>
+    <t>MOTOR TRICYCLE (TUK TUK)</t>
+  </si>
+  <si>
+    <t>MAXPAC PERSONAL ACCIDENT</t>
+  </si>
+  <si>
+    <t>MOTOR PSV (MUASALAT)</t>
+  </si>
+  <si>
+    <t>MOTOR CYCLE (BODA BODA)</t>
+  </si>
+  <si>
+    <t>0000012198</t>
+  </si>
+  <si>
+    <t>0000012202</t>
   </si>
 </sst>
 </file>
@@ -1146,7 +1201,7 @@
   <dimension ref="A1:A19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1210,10 +1265,14 @@
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" s="6"/>
+      <c r="A12" s="6" t="s">
+        <v>252</v>
+      </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" s="6"/>
+      <c r="A13" s="6" t="s">
+        <v>253</v>
+      </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" s="6"/>
@@ -1243,7 +1302,7 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1263,15 +1322,15 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>225</v>
+        <v>238</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>218</v>
+        <v>236</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>159</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -1334,7 +1393,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F06FDF89-FCC4-438E-B054-39500F380DC7}">
           <x14:formula1>
-            <xm:f>valid_product_names!$A$1:$E$1</xm:f>
+            <xm:f>valid_product_names!$A$1:$F$1</xm:f>
           </x14:formula1>
           <xm:sqref>C2</xm:sqref>
         </x14:dataValidation>
@@ -1346,10 +1405,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35D5C44B-F88A-4340-B982-5E1C9A94327D}">
-  <dimension ref="A1:E62"/>
+  <dimension ref="A1:F62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" activeCellId="4" sqref="A1:A62 B1:B62 C1:C51 A1:D54 E1:E16"/>
+      <selection activeCell="F1" activeCellId="5" sqref="A1:A62 B1:B62 C1:C51 D1:D54 E1:E16 F1:F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1360,7 +1419,7 @@
     <col min="4" max="4" width="33.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>63</v>
       </c>
@@ -1376,8 +1435,11 @@
       <c r="E1" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1393,8 +1455,11 @@
       <c r="E2" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1410,8 +1475,11 @@
       <c r="E3" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1427,8 +1495,11 @@
       <c r="E4" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4" s="4" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1444,8 +1515,11 @@
       <c r="E5" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -1461,8 +1535,11 @@
       <c r="E6" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F6" s="4" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -1478,8 +1555,11 @@
       <c r="E7" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F7" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -1495,8 +1575,11 @@
       <c r="E8" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F8" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1512,8 +1595,11 @@
       <c r="E9" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F9" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -1529,8 +1615,11 @@
       <c r="E10" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F10" s="4" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1546,8 +1635,11 @@
       <c r="E11" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F11" s="4" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1563,8 +1655,11 @@
       <c r="E12" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F12" s="4" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1580,8 +1675,11 @@
       <c r="E13" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F13" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1597,8 +1695,11 @@
       <c r="E14" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F14" s="4" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -1614,8 +1715,11 @@
       <c r="E15" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F15" s="4" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -1631,8 +1735,11 @@
       <c r="E16" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F16" s="4" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -1645,8 +1752,11 @@
       <c r="D17" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F17" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -1659,8 +1769,11 @@
       <c r="D18" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F18" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -1673,8 +1786,11 @@
       <c r="D19" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F19" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -1687,8 +1803,11 @@
       <c r="D20" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F20" s="4" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -1701,8 +1820,11 @@
       <c r="D21" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F21" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -1715,8 +1837,11 @@
       <c r="D22" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F22" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -1729,8 +1854,11 @@
       <c r="D23" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F23" s="4" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -1743,8 +1871,11 @@
       <c r="D24" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F24" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -1757,8 +1888,11 @@
       <c r="D25" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F25" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -1771,8 +1905,11 @@
       <c r="D26" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F26" s="4" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -1785,8 +1922,11 @@
       <c r="D27" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F27" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -1799,8 +1939,11 @@
       <c r="D28" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F28" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -1813,8 +1956,11 @@
       <c r="D29" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F29" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -1827,8 +1973,11 @@
       <c r="D30" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F30" s="4" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -1841,8 +1990,11 @@
       <c r="D31" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F31" s="4" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>32</v>
       </c>
@@ -1855,8 +2007,11 @@
       <c r="D32" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F32" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>33</v>
       </c>
@@ -1869,8 +2024,11 @@
       <c r="D33" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F33" s="4" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>34</v>
       </c>
@@ -1883,8 +2041,11 @@
       <c r="D34" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F34" s="4" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>35</v>
       </c>
@@ -1897,8 +2058,11 @@
       <c r="D35" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F35" s="4" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -1912,7 +2076,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>37</v>
       </c>
@@ -1926,7 +2090,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>38</v>
       </c>
@@ -1940,7 +2104,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>39</v>
       </c>
@@ -1954,7 +2118,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>40</v>
       </c>
@@ -1968,7 +2132,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>41</v>
       </c>
@@ -1982,7 +2146,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>42</v>
       </c>
@@ -1996,7 +2160,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>43</v>
       </c>
@@ -2010,7 +2174,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>44</v>
       </c>
@@ -2024,7 +2188,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>45</v>
       </c>
@@ -2038,7 +2202,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>46</v>
       </c>
@@ -2052,7 +2216,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>47</v>
       </c>
@@ -2066,7 +2230,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>48</v>
       </c>

</xml_diff>

<commit_message>
Excluded life products following feedback by Rachel and cokey.
</commit_message>
<xml_diff>
--- a/App/uap_cross_sell/www/files/cs_upload_template.xlsx
+++ b/App/uap_cross_sell/www/files/cs_upload_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tayojabar/Documents/OML/UAP-cross-sell/UAP-cross-sell/App/uap_cross_sell/www/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Contracts\UAP\D - Working Papers\UAP-cross-sell\App\uap_cross_sell\www\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE4AE1CC-D5E9-4F43-A84C-30DF25AA8578}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AF16627-7518-426B-AEDF-421BCF7273DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{24700C77-9C92-4468-B9C5-B77420552ACF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{24700C77-9C92-4468-B9C5-B77420552ACF}"/>
   </bookViews>
   <sheets>
     <sheet name="customer_acc" sheetId="1" r:id="rId1"/>
@@ -19,10 +19,10 @@
   </sheets>
   <definedNames>
     <definedName name="Ghana">valid_product_names!$E$2:$E$16</definedName>
-    <definedName name="Kenya">valid_product_names!$A$2:$A$54</definedName>
-    <definedName name="Nigeria">valid_product_names!$D$2:$D$54</definedName>
-    <definedName name="Uganda">valid_product_names!$C$2:$C$54</definedName>
-    <definedName name="Zimbabwe">valid_product_names!$B$2:$B$54</definedName>
+    <definedName name="Kenya">valid_product_names!$A$2:$A$62</definedName>
+    <definedName name="Nigeria">valid_product_names!$D$2:$D$38</definedName>
+    <definedName name="Uganda">valid_product_names!$C$2:$C$51</definedName>
+    <definedName name="Zimbabwe">valid_product_names!$B$2:$B$62</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="222">
   <si>
     <t>Old Mutual Equity Fund</t>
   </si>
@@ -543,54 +543,6 @@
     <t>Nigeria</t>
   </si>
   <si>
-    <t>Savings Product</t>
-  </si>
-  <si>
-    <t>Family Risk Product</t>
-  </si>
-  <si>
-    <t>Life Product</t>
-  </si>
-  <si>
-    <t>GROUP LIFE ONLY</t>
-  </si>
-  <si>
-    <t>CREDIT LIFE ASSURANCE</t>
-  </si>
-  <si>
-    <t>INVESTMENT LINK SCHEME</t>
-  </si>
-  <si>
-    <t>OCEANIC EDUCATION ASSURANCE POLICY</t>
-  </si>
-  <si>
-    <t>OCEANFLEX CONTRIBUTION ASS. SCHEME</t>
-  </si>
-  <si>
-    <t>OCEANTAP</t>
-  </si>
-  <si>
-    <t>OCEANIC EDUCATION ASSURANCE POLICY1</t>
-  </si>
-  <si>
-    <t>CREDIT LIFE ASSURANCE 2</t>
-  </si>
-  <si>
-    <t>TERM ASSURANCE</t>
-  </si>
-  <si>
-    <t>TERM ASS. WITH REFUND</t>
-  </si>
-  <si>
-    <t>MORTGAGE PROTECTION SCHEME</t>
-  </si>
-  <si>
-    <t>OCEANIC BABY PLAN</t>
-  </si>
-  <si>
-    <t>NATA</t>
-  </si>
-  <si>
     <t>Public Liability (not energy Risks)</t>
   </si>
   <si>
@@ -742,13 +694,19 @@
   </si>
   <si>
     <t>AS000883</t>
+  </si>
+  <si>
+    <t>3013483433</t>
+  </si>
+  <si>
+    <t>3013460492</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1146,91 +1104,95 @@
   <dimension ref="A1:A19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" s="1" customFormat="1">
       <c r="A1" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1">
       <c r="A2" s="6">
         <v>1537</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1">
       <c r="A3" s="6">
         <v>1418</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1">
       <c r="A4" s="6">
         <v>100003</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1">
       <c r="A5" s="6">
         <v>101403</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1">
       <c r="A6" s="6">
         <v>1016908</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:1">
       <c r="A7" s="6">
         <v>1024783</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:1">
       <c r="A8" s="6">
         <v>1016764</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:1">
       <c r="A9" s="6">
         <v>1023406</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:1">
       <c r="A10" s="6" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
       <c r="A11" s="6" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" s="6"/>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" s="6"/>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" s="6" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" s="6" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
       <c r="A14" s="6"/>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:1">
       <c r="A15" s="6"/>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:1">
       <c r="A16" s="6"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1">
       <c r="A17" s="6"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1">
       <c r="A18" s="6"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1">
       <c r="A19" s="6"/>
     </row>
   </sheetData>
@@ -1243,17 +1205,17 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="34.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" s="1" customFormat="1">
       <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
@@ -1261,65 +1223,65 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>225</v>
+        <v>170</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="2"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="A5" s="2"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3">
       <c r="A6" s="2"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3">
       <c r="A7" s="2"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3">
       <c r="A8" s="2"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3">
       <c r="A9" s="2"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3">
       <c r="A10" s="2"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3">
       <c r="A11" s="2"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3">
       <c r="A12" s="2"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3">
       <c r="A13" s="2"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3">
       <c r="A14" s="2"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3">
       <c r="A15" s="2"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3">
       <c r="A16" s="2"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1">
       <c r="A17" s="2"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1">
       <c r="A18" s="2"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1">
       <c r="A19" s="2"/>
     </row>
   </sheetData>
@@ -1349,18 +1311,18 @@
   <dimension ref="A1:E62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" activeCellId="4" sqref="A1:A62 B1:B62 C1:C51 A1:D54 E1:E16"/>
+      <selection activeCell="E1" activeCellId="4" sqref="A1:A62 B1:B62 C1:C51 D1:D38 E1:E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="37" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="54.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="56.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="56.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>63</v>
       </c>
@@ -1374,10 +1336,10 @@
         <v>168</v>
       </c>
       <c r="E1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1391,10 +1353,10 @@
         <v>169</v>
       </c>
       <c r="E2" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1408,10 +1370,10 @@
         <v>170</v>
       </c>
       <c r="E3" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1425,10 +1387,10 @@
         <v>171</v>
       </c>
       <c r="E4" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1442,10 +1404,10 @@
         <v>172</v>
       </c>
       <c r="E5" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -1459,10 +1421,10 @@
         <v>173</v>
       </c>
       <c r="E6" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -1476,10 +1438,10 @@
         <v>174</v>
       </c>
       <c r="E7" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -1493,10 +1455,10 @@
         <v>175</v>
       </c>
       <c r="E8" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1510,10 +1472,10 @@
         <v>176</v>
       </c>
       <c r="E9" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -1527,10 +1489,10 @@
         <v>177</v>
       </c>
       <c r="E10" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1544,10 +1506,10 @@
         <v>178</v>
       </c>
       <c r="E11" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1561,10 +1523,10 @@
         <v>179</v>
       </c>
       <c r="E12" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1578,10 +1540,10 @@
         <v>180</v>
       </c>
       <c r="E13" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1595,10 +1557,10 @@
         <v>181</v>
       </c>
       <c r="E14" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -1612,10 +1574,10 @@
         <v>182</v>
       </c>
       <c r="E15" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -1629,10 +1591,10 @@
         <v>183</v>
       </c>
       <c r="E16" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -1646,7 +1608,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -1657,10 +1619,10 @@
         <v>32</v>
       </c>
       <c r="D18" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -1671,10 +1633,10 @@
         <v>130</v>
       </c>
       <c r="D19" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -1685,10 +1647,10 @@
         <v>131</v>
       </c>
       <c r="D20" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -1699,10 +1661,10 @@
         <v>132</v>
       </c>
       <c r="D21" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -1713,10 +1675,10 @@
         <v>133</v>
       </c>
       <c r="D22" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -1727,10 +1689,10 @@
         <v>134</v>
       </c>
       <c r="D23" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -1741,10 +1703,10 @@
         <v>135</v>
       </c>
       <c r="D24" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -1755,10 +1717,10 @@
         <v>136</v>
       </c>
       <c r="D25" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -1769,10 +1731,10 @@
         <v>30</v>
       </c>
       <c r="D26" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -1783,10 +1745,10 @@
         <v>137</v>
       </c>
       <c r="D27" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -1797,10 +1759,10 @@
         <v>138</v>
       </c>
       <c r="D28" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -1811,10 +1773,10 @@
         <v>146</v>
       </c>
       <c r="D29" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -1825,10 +1787,10 @@
         <v>41</v>
       </c>
       <c r="D30" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -1839,10 +1801,10 @@
         <v>28</v>
       </c>
       <c r="D31" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
       <c r="A32" t="s">
         <v>32</v>
       </c>
@@ -1853,10 +1815,10 @@
         <v>140</v>
       </c>
       <c r="D32" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
       <c r="A33" t="s">
         <v>33</v>
       </c>
@@ -1867,10 +1829,10 @@
         <v>141</v>
       </c>
       <c r="D33" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
       <c r="A34" t="s">
         <v>34</v>
       </c>
@@ -1881,10 +1843,10 @@
         <v>142</v>
       </c>
       <c r="D34" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
       <c r="A35" t="s">
         <v>35</v>
       </c>
@@ -1895,10 +1857,10 @@
         <v>143</v>
       </c>
       <c r="D35" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -1909,10 +1871,10 @@
         <v>144</v>
       </c>
       <c r="D36" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
       <c r="A37" t="s">
         <v>37</v>
       </c>
@@ -1923,10 +1885,10 @@
         <v>145</v>
       </c>
       <c r="D37" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
       <c r="A38" t="s">
         <v>38</v>
       </c>
@@ -1937,10 +1899,10 @@
         <v>151</v>
       </c>
       <c r="D38" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
       <c r="A39" t="s">
         <v>39</v>
       </c>
@@ -1950,11 +1912,8 @@
       <c r="C39" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="D39" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="1:4">
       <c r="A40" t="s">
         <v>40</v>
       </c>
@@ -1964,11 +1923,8 @@
       <c r="C40" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="D40" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="41" spans="1:4">
       <c r="A41" t="s">
         <v>41</v>
       </c>
@@ -1978,11 +1934,8 @@
       <c r="C41" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="D41" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="42" spans="1:4">
       <c r="A42" t="s">
         <v>42</v>
       </c>
@@ -1992,11 +1945,8 @@
       <c r="C42" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="D42" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="43" spans="1:4">
       <c r="A43" t="s">
         <v>43</v>
       </c>
@@ -2006,11 +1956,8 @@
       <c r="C43" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="D43" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="44" spans="1:4">
       <c r="A44" t="s">
         <v>44</v>
       </c>
@@ -2020,11 +1967,8 @@
       <c r="C44" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="D44" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="45" spans="1:4">
       <c r="A45" t="s">
         <v>45</v>
       </c>
@@ -2034,11 +1978,8 @@
       <c r="C45" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="D45" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="46" spans="1:4">
       <c r="A46" t="s">
         <v>46</v>
       </c>
@@ -2048,11 +1989,8 @@
       <c r="C46" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="D46" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="47" spans="1:4">
       <c r="A47" t="s">
         <v>47</v>
       </c>
@@ -2062,11 +2000,8 @@
       <c r="C47" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D47" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="48" spans="1:4">
       <c r="A48" t="s">
         <v>48</v>
       </c>
@@ -2076,11 +2011,8 @@
       <c r="C48" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="D48" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="49" spans="1:3">
       <c r="A49" t="s">
         <v>49</v>
       </c>
@@ -2090,11 +2022,8 @@
       <c r="C49" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="D49" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="50" spans="1:3">
       <c r="A50" t="s">
         <v>50</v>
       </c>
@@ -2104,11 +2033,8 @@
       <c r="C50" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="D50" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="51" spans="1:3">
       <c r="A51" t="s">
         <v>51</v>
       </c>
@@ -2118,44 +2044,32 @@
       <c r="C51" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="D51" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="52" spans="1:3">
       <c r="A52" t="s">
         <v>52</v>
       </c>
       <c r="B52" t="s">
         <v>111</v>
       </c>
-      <c r="D52" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="53" spans="1:3">
       <c r="A53" t="s">
         <v>53</v>
       </c>
       <c r="B53" t="s">
         <v>112</v>
       </c>
-      <c r="D53" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="54" spans="1:3">
       <c r="A54" t="s">
         <v>54</v>
       </c>
       <c r="B54" t="s">
         <v>113</v>
       </c>
-      <c r="D54" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="55" spans="1:3">
       <c r="A55" t="s">
         <v>55</v>
       </c>
@@ -2163,7 +2077,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:3">
       <c r="A56" t="s">
         <v>56</v>
       </c>
@@ -2171,7 +2085,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:3">
       <c r="A57" t="s">
         <v>57</v>
       </c>
@@ -2179,7 +2093,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:3">
       <c r="A58" t="s">
         <v>58</v>
       </c>
@@ -2187,7 +2101,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:3">
       <c r="A59" t="s">
         <v>59</v>
       </c>
@@ -2195,7 +2109,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:3">
       <c r="A60" t="s">
         <v>60</v>
       </c>
@@ -2203,7 +2117,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:3">
       <c r="A61" t="s">
         <v>61</v>
       </c>
@@ -2211,7 +2125,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:3">
       <c r="A62" t="s">
         <v>62</v>
       </c>

</xml_diff>

<commit_message>
Bulk upload template with all countries.
</commit_message>
<xml_diff>
--- a/App/uap_cross_sell/www/files/cs_upload_template.xlsx
+++ b/App/uap_cross_sell/www/files/cs_upload_template.xlsx
@@ -1,29 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tayojabar/Documents/OML/UAP-cross-sell/UAP-cross-sell/App/uap_cross_sell/www/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Contracts\UAP\D - Working Papers\UAP-cross-sell\App\uap_cross_sell\www\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1535B10-8D2E-8C46-9220-0252849C5600}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA7FE19C-A639-420A-A066-0D798902CB67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16440" activeTab="1" xr2:uid="{24700C77-9C92-4468-B9C5-B77420552ACF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{24700C77-9C92-4468-B9C5-B77420552ACF}"/>
   </bookViews>
   <sheets>
     <sheet name="customer_acc" sheetId="1" r:id="rId1"/>
     <sheet name="customer_prod" sheetId="2" r:id="rId2"/>
-    <sheet name="valid_product_names" sheetId="3" r:id="rId3"/>
+    <sheet name="valid_product_names" sheetId="3" state="hidden" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="Ghana">valid_product_names!$E$2:$E$16</definedName>
     <definedName name="Kenya">valid_product_names!$A$2:$A$62</definedName>
-    <definedName name="Nigeria">valid_product_names!$D$2:$D$54</definedName>
+    <definedName name="Nigeria">valid_product_names!$D$2:$D$38</definedName>
     <definedName name="Sudan">valid_product_names!$F$2:$F$37</definedName>
     <definedName name="Uganda">valid_product_names!$C$2:$C$51</definedName>
-    <definedName name="Zimbabwe">valid_product_names!$B$2:$B$62</definedName>
+    <definedName name="Zimbabwe">valid_product_names!$B$2:$B$89</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="267">
   <si>
     <t>Old Mutual Equity Fund</t>
   </si>
@@ -544,54 +544,6 @@
     <t>Nigeria</t>
   </si>
   <si>
-    <t>Savings Product</t>
-  </si>
-  <si>
-    <t>Family Risk Product</t>
-  </si>
-  <si>
-    <t>Life Product</t>
-  </si>
-  <si>
-    <t>GROUP LIFE ONLY</t>
-  </si>
-  <si>
-    <t>CREDIT LIFE ASSURANCE</t>
-  </si>
-  <si>
-    <t>INVESTMENT LINK SCHEME</t>
-  </si>
-  <si>
-    <t>OCEANIC EDUCATION ASSURANCE POLICY</t>
-  </si>
-  <si>
-    <t>OCEANFLEX CONTRIBUTION ASS. SCHEME</t>
-  </si>
-  <si>
-    <t>OCEANTAP</t>
-  </si>
-  <si>
-    <t>OCEANIC EDUCATION ASSURANCE POLICY1</t>
-  </si>
-  <si>
-    <t>CREDIT LIFE ASSURANCE 2</t>
-  </si>
-  <si>
-    <t>TERM ASSURANCE</t>
-  </si>
-  <si>
-    <t>TERM ASS. WITH REFUND</t>
-  </si>
-  <si>
-    <t>MORTGAGE PROTECTION SCHEME</t>
-  </si>
-  <si>
-    <t>OCEANIC BABY PLAN</t>
-  </si>
-  <si>
-    <t>NATA</t>
-  </si>
-  <si>
     <t>Public Liability (not energy Risks)</t>
   </si>
   <si>
@@ -742,9 +694,6 @@
     <t>AG002068</t>
   </si>
   <si>
-    <t>AS000883</t>
-  </si>
-  <si>
     <t>Sudan</t>
   </si>
   <si>
@@ -796,14 +745,104 @@
     <t>0000012198</t>
   </si>
   <si>
-    <t>0000012202</t>
+    <t>Blue Nostro FCA</t>
+  </si>
+  <si>
+    <t>Nostro FCA</t>
+  </si>
+  <si>
+    <t>Blue Current Account - RTGS$</t>
+  </si>
+  <si>
+    <t>Blue Savings Account - RTGS FCA</t>
+  </si>
+  <si>
+    <t>Gold Current Account - RTGS$</t>
+  </si>
+  <si>
+    <t>Gold Nostro FCA</t>
+  </si>
+  <si>
+    <t>MasterCard Nostro FCA</t>
+  </si>
+  <si>
+    <t>Mortgage Loan</t>
+  </si>
+  <si>
+    <t>Loans</t>
+  </si>
+  <si>
+    <t>Personal Loans</t>
+  </si>
+  <si>
+    <t>Platinum Current Account - RTGS$</t>
+  </si>
+  <si>
+    <t>Platinum Nostro FCA</t>
+  </si>
+  <si>
+    <t>Textacash Nostro FCA</t>
+  </si>
+  <si>
+    <t>Gold Savings Account - RTGS FCA</t>
+  </si>
+  <si>
+    <t>Home Loans</t>
+  </si>
+  <si>
+    <t>Overdraft</t>
+  </si>
+  <si>
+    <t>Platinum Savings Acc - RTGS FCA</t>
+  </si>
+  <si>
+    <t>Short term Loans (&lt;/= yr)</t>
+  </si>
+  <si>
+    <t>Term Loans (&gt; 1 YR)</t>
+  </si>
+  <si>
+    <t>Term Deposits Takings</t>
+  </si>
+  <si>
+    <t>Nostro Equity Release loans</t>
+  </si>
+  <si>
+    <t>Vehicle Loan</t>
+  </si>
+  <si>
+    <t>Negotiable Loan</t>
+  </si>
+  <si>
+    <t>Nostro 'Short term Loans (&lt;/= yr)'</t>
+  </si>
+  <si>
+    <t>Nostro Term Loans (&gt; 1 YR)</t>
+  </si>
+  <si>
+    <t>textacash</t>
+  </si>
+  <si>
+    <t>ewallet</t>
+  </si>
+  <si>
+    <t>0000013188</t>
+  </si>
+  <si>
+    <t>3013656028</t>
+  </si>
+  <si>
+    <t>1418</t>
+  </si>
+  <si>
+    <t>1125981741</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -834,7 +873,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -844,6 +883,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -875,7 +920,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -884,6 +929,7 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1198,99 +1244,70 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C783F41-9AF8-4698-A4E2-A0CDF8EF2C34}">
-  <dimension ref="A1:A19"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" s="1" customFormat="1">
       <c r="A1" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6">
-        <v>1537</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="6">
-        <v>1418</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="6">
-        <v>100003</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="6">
-        <v>101403</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="6">
-        <v>1016908</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" s="6">
-        <v>1024783</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" s="6">
-        <v>1016764</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" s="6">
-        <v>1023406</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" s="6" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
+    <row r="2" spans="1:3">
+      <c r="A2" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="C2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="C3" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="6" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" s="6" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" s="6" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A14" s="6"/>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A15" s="6"/>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A16" s="6"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="6"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="6"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="6"/>
+      <c r="C4" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="6" t="s">
+        <v>263</v>
+      </c>
+      <c r="C5" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="8" t="s">
+        <v>266</v>
+      </c>
+      <c r="C6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="6" t="s">
+        <v>264</v>
+      </c>
+      <c r="C7" t="s">
+        <v>168</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1301,18 +1318,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A24E3401-6C35-4108-BA35-AB6F39FFE1F7}">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="34.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" s="1" customFormat="1">
       <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
@@ -1320,65 +1337,65 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="2"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="A5" s="2"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3">
       <c r="A6" s="2"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3">
       <c r="A7" s="2"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3">
       <c r="A8" s="2"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3">
       <c r="A9" s="2"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3">
       <c r="A10" s="2"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3">
       <c r="A11" s="2"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3">
       <c r="A12" s="2"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3">
       <c r="A13" s="2"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3">
       <c r="A14" s="2"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3">
       <c r="A15" s="2"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3">
       <c r="A16" s="2"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1">
       <c r="A17" s="2"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1">
       <c r="A18" s="2"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1">
       <c r="A19" s="2"/>
     </row>
   </sheetData>
@@ -1405,21 +1422,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35D5C44B-F88A-4340-B982-5E1C9A94327D}">
-  <dimension ref="A1:F62"/>
+  <dimension ref="A1:F89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" activeCellId="5" sqref="A1:A62 B1:B62 C1:C51 D1:D54 E1:E16 F1:F37"/>
+      <selection activeCell="F1" activeCellId="5" sqref="A1:A62 B1:B89 C1:C51 D1:D38 E1:E16 F1:F37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="37" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="54.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="56.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="41.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>63</v>
       </c>
@@ -1433,18 +1452,18 @@
         <v>168</v>
       </c>
       <c r="E1" t="s">
-        <v>218</v>
+        <v>202</v>
       </c>
       <c r="F1" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>67</v>
+        <v>236</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>158</v>
@@ -1453,18 +1472,18 @@
         <v>169</v>
       </c>
       <c r="E2" t="s">
-        <v>219</v>
+        <v>203</v>
       </c>
       <c r="F2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>153</v>
+        <v>237</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>3</v>
@@ -1473,18 +1492,18 @@
         <v>170</v>
       </c>
       <c r="E3" t="s">
-        <v>220</v>
+        <v>204</v>
       </c>
       <c r="F3" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>74</v>
+        <v>238</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>159</v>
@@ -1493,18 +1512,18 @@
         <v>171</v>
       </c>
       <c r="E4" t="s">
-        <v>221</v>
+        <v>205</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>75</v>
+        <v>239</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>160</v>
@@ -1513,18 +1532,18 @@
         <v>172</v>
       </c>
       <c r="E5" t="s">
-        <v>222</v>
+        <v>206</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>22</v>
@@ -1533,18 +1552,18 @@
         <v>173</v>
       </c>
       <c r="E6" t="s">
-        <v>223</v>
+        <v>207</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>154</v>
+        <v>67</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>27</v>
@@ -1553,18 +1572,18 @@
         <v>174</v>
       </c>
       <c r="E7" t="s">
-        <v>224</v>
+        <v>208</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>155</v>
+        <v>240</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>123</v>
@@ -1573,18 +1592,18 @@
         <v>175</v>
       </c>
       <c r="E8" t="s">
-        <v>225</v>
+        <v>209</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>156</v>
+        <v>241</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>139</v>
@@ -1593,18 +1612,18 @@
         <v>176</v>
       </c>
       <c r="E9" t="s">
-        <v>226</v>
+        <v>210</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>157</v>
+        <v>242</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>26</v>
@@ -1613,18 +1632,18 @@
         <v>177</v>
       </c>
       <c r="E10" t="s">
-        <v>227</v>
+        <v>211</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>77</v>
+        <v>243</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>129</v>
@@ -1633,18 +1652,18 @@
         <v>178</v>
       </c>
       <c r="E11" t="s">
-        <v>228</v>
+        <v>212</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>124</v>
@@ -1653,18 +1672,18 @@
         <v>179</v>
       </c>
       <c r="E12" t="s">
-        <v>229</v>
+        <v>213</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>70</v>
+        <v>244</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>125</v>
@@ -1673,18 +1692,18 @@
         <v>180</v>
       </c>
       <c r="E13" t="s">
-        <v>230</v>
+        <v>214</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>126</v>
@@ -1693,18 +1712,18 @@
         <v>181</v>
       </c>
       <c r="E14" t="s">
-        <v>231</v>
+        <v>215</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>127</v>
@@ -1713,18 +1732,18 @@
         <v>182</v>
       </c>
       <c r="E15" t="s">
-        <v>232</v>
+        <v>216</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>65</v>
+        <v>245</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>128</v>
@@ -1733,18 +1752,18 @@
         <v>183</v>
       </c>
       <c r="E16" t="s">
-        <v>233</v>
+        <v>217</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>64</v>
+        <v>246</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>29</v>
@@ -1753,640 +1772,727 @@
         <v>184</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>66</v>
+        <v>247</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>32</v>
       </c>
       <c r="D18" t="s">
-        <v>185</v>
+        <v>110</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>78</v>
+        <v>248</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>130</v>
       </c>
       <c r="D19" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>79</v>
+        <v>249</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>131</v>
       </c>
       <c r="D20" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
         <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>80</v>
+        <v>250</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>132</v>
       </c>
       <c r="D21" t="s">
-        <v>188</v>
+        <v>84</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>133</v>
       </c>
       <c r="D22" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" t="s">
         <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>82</v>
+        <v>153</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>134</v>
       </c>
       <c r="D23" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F23" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
         <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>83</v>
+        <v>154</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>135</v>
       </c>
       <c r="D24" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F24" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6">
       <c r="A25" t="s">
         <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>84</v>
+        <v>251</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>136</v>
       </c>
       <c r="D25" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
         <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D26" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="F26" s="4" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
         <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>86</v>
+        <v>252</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>137</v>
       </c>
       <c r="D27" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F27" s="4" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6">
       <c r="A28" t="s">
         <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>87</v>
+        <v>253</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>138</v>
       </c>
       <c r="D28" t="s">
-        <v>195</v>
+        <v>99</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29" t="s">
         <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>88</v>
+        <v>254</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>146</v>
       </c>
       <c r="D29" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="F29" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6">
       <c r="A30" t="s">
         <v>30</v>
       </c>
       <c r="B30" t="s">
-        <v>89</v>
+        <v>155</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>41</v>
       </c>
       <c r="D30" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="F30" s="4" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6">
       <c r="A31" t="s">
         <v>31</v>
       </c>
       <c r="B31" t="s">
-        <v>90</v>
+        <v>255</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>28</v>
       </c>
       <c r="D31" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="F31" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6">
       <c r="A32" t="s">
         <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>140</v>
       </c>
       <c r="D32" t="s">
-        <v>199</v>
+        <v>91</v>
       </c>
       <c r="F32" s="4" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6">
       <c r="A33" t="s">
         <v>33</v>
       </c>
       <c r="B33" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>141</v>
       </c>
       <c r="D33" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
       <c r="A34" t="s">
         <v>34</v>
       </c>
       <c r="B34" t="s">
-        <v>93</v>
+        <v>256</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>142</v>
       </c>
       <c r="D34" t="s">
-        <v>110</v>
+        <v>197</v>
       </c>
       <c r="F34" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6">
       <c r="A35" t="s">
         <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>94</v>
+        <v>65</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>143</v>
       </c>
       <c r="D35" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
       <c r="A36" t="s">
         <v>36</v>
       </c>
       <c r="B36" t="s">
-        <v>95</v>
+        <v>64</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>144</v>
       </c>
       <c r="D36" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
       <c r="A37" t="s">
         <v>37</v>
       </c>
       <c r="B37" t="s">
-        <v>96</v>
+        <v>66</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>145</v>
       </c>
       <c r="D37" t="s">
-        <v>84</v>
+        <v>200</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
       <c r="A38" t="s">
         <v>38</v>
       </c>
       <c r="B38" t="s">
-        <v>97</v>
+        <v>78</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>151</v>
       </c>
       <c r="D38" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
       <c r="A39" t="s">
         <v>39</v>
       </c>
       <c r="B39" t="s">
-        <v>98</v>
+        <v>79</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="D39" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="1:6">
       <c r="A40" t="s">
         <v>40</v>
       </c>
       <c r="B40" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="D40" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="41" spans="1:6">
       <c r="A41" t="s">
         <v>41</v>
       </c>
       <c r="B41" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="D41" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="42" spans="1:6">
       <c r="A42" t="s">
         <v>42</v>
       </c>
       <c r="B42" t="s">
-        <v>101</v>
+        <v>82</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="D42" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="43" spans="1:6">
       <c r="A43" t="s">
         <v>43</v>
       </c>
       <c r="B43" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="D43" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="44" spans="1:6">
       <c r="A44" t="s">
         <v>44</v>
       </c>
       <c r="B44" t="s">
-        <v>103</v>
+        <v>84</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="D44" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="45" spans="1:6">
       <c r="A45" t="s">
         <v>45</v>
       </c>
       <c r="B45" t="s">
-        <v>104</v>
+        <v>85</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="D45" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="46" spans="1:6">
       <c r="A46" t="s">
         <v>46</v>
       </c>
       <c r="B46" t="s">
-        <v>105</v>
+        <v>86</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="D46" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="47" spans="1:6">
       <c r="A47" t="s">
         <v>47</v>
       </c>
       <c r="B47" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D47" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="48" spans="1:6">
       <c r="A48" t="s">
         <v>48</v>
       </c>
       <c r="B48" t="s">
-        <v>107</v>
+        <v>88</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="D48" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="49" spans="1:3">
       <c r="A49" t="s">
         <v>49</v>
       </c>
       <c r="B49" t="s">
-        <v>108</v>
+        <v>89</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="D49" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="50" spans="1:3">
       <c r="A50" t="s">
         <v>50</v>
       </c>
       <c r="B50" t="s">
-        <v>109</v>
+        <v>90</v>
       </c>
       <c r="C50" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="D50" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="51" spans="1:3">
       <c r="A51" t="s">
         <v>51</v>
       </c>
       <c r="B51" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="C51" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="D51" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="52" spans="1:3">
       <c r="A52" t="s">
         <v>52</v>
       </c>
       <c r="B52" t="s">
-        <v>111</v>
-      </c>
-      <c r="D52" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
       <c r="A53" t="s">
         <v>53</v>
       </c>
       <c r="B53" t="s">
-        <v>112</v>
-      </c>
-      <c r="D53" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
       <c r="A54" t="s">
         <v>54</v>
       </c>
       <c r="B54" t="s">
-        <v>113</v>
-      </c>
-      <c r="D54" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
       <c r="A55" t="s">
         <v>55</v>
       </c>
       <c r="B55" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
       <c r="A56" t="s">
         <v>56</v>
       </c>
       <c r="B56" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
       <c r="A57" t="s">
         <v>57</v>
       </c>
       <c r="B57" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
       <c r="A58" t="s">
         <v>58</v>
       </c>
       <c r="B58" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
       <c r="A59" t="s">
         <v>59</v>
       </c>
       <c r="B59" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
       <c r="A60" t="s">
         <v>60</v>
       </c>
       <c r="B60" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
       <c r="A61" t="s">
         <v>61</v>
       </c>
       <c r="B61" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
       <c r="A62" t="s">
         <v>62</v>
       </c>
       <c r="B62" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="B63" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="B64" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2">
+      <c r="B65" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2">
+      <c r="B66" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="67" spans="2:2">
+      <c r="B67" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="68" spans="2:2">
+      <c r="B68" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="69" spans="2:2">
+      <c r="B69" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="70" spans="2:2">
+      <c r="B70" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="71" spans="2:2">
+      <c r="B71" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="72" spans="2:2">
+      <c r="B72" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="73" spans="2:2">
+      <c r="B73" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="74" spans="2:2">
+      <c r="B74" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="75" spans="2:2">
+      <c r="B75" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="76" spans="2:2">
+      <c r="B76" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="77" spans="2:2">
+      <c r="B77" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="78" spans="2:2">
+      <c r="B78" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="79" spans="2:2">
+      <c r="B79" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="80" spans="2:2">
+      <c r="B80" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="81" spans="2:2">
+      <c r="B81" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="82" spans="2:2">
+      <c r="B82" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="83" spans="2:2">
+      <c r="B83" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="84" spans="2:2">
+      <c r="B84" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="85" spans="2:2">
+      <c r="B85" t="s">
         <v>121</v>
+      </c>
+    </row>
+    <row r="86" spans="2:2">
+      <c r="B86" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="87" spans="2:2">
+      <c r="B87" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="88" spans="2:2">
+      <c r="B88" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="89" spans="2:2">
+      <c r="B89" t="s">
+        <v>262</v>
       </c>
     </row>
   </sheetData>

</xml_diff>